<commit_message>
conf 에 mergeCells 추가.
</commit_message>
<xml_diff>
--- a/test/testExcel.xlsx
+++ b/test/testExcel.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
   <si>
-    <t>해더1-1722325964</t>
+    <t>해더1-1722391550</t>
   </si>
   <si>
     <t>해더2</t>
@@ -770,9 +770,7 @@
       <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
-        <v>4</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2">
         <v>5</v>
       </c>
@@ -909,6 +907,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId_hyperlink_1"/>
     <hyperlink ref="B4" r:id="rId_hyperlink_2"/>

</xml_diff>